<commit_message>
atualiza registro de peca e config e-mail
</commit_message>
<xml_diff>
--- a/pedidos.xlsx
+++ b/pedidos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -480,6 +480,95 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>2024-09-04 17:18:27</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr"/>
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="n">
+        <v>238001</v>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>kit roletes</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2024-09-04 17:24:19</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr"/>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="n">
+        <v>238001</v>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>kit roletes</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2024-09-04</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>17:28:07</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>X3BK036141</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>WF-M5799</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>EPSON</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>BL. A (3º) - UTI A PST 3</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>10.16.13.143</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>238001</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>kit roletes</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>